<commit_message>
se realiza mapeo de objetos correspondientes al login
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/autenticacion/autenticacion.xlsx
+++ b/SVP/src/test/resources/datadriven/autenticacion/autenticacion.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="26311"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mruiz/Documents/ProyectosTODO1/svp-rediseno-personas-web-tests-bdd-screenplay/SVP/src/test/resources/datadriven/autenticacion/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="13080"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
     <sheet name="Listas" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>Orientacion</t>
   </si>
@@ -88,13 +83,16 @@
   </si>
   <si>
     <t>7</t>
+  </si>
+  <si>
+    <t>SVPPRU08</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -474,7 +472,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -485,24 +483,24 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -534,7 +532,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -545,12 +543,16 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="1"/>
+      <c r="G2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1234</v>
+      </c>
       <c r="I2" s="1"/>
       <c r="J2" s="4"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
@@ -566,7 +568,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="4"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
@@ -582,7 +584,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="4"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
@@ -598,7 +600,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
@@ -614,7 +616,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="4"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10">
       <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
@@ -630,7 +632,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="A8" s="4" t="s">
         <v>19</v>
       </c>
@@ -670,19 +672,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Se implementan script de la HU Autenticación eestos no cubren la funcionalida completa
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/autenticacion/autenticacion.xlsx
+++ b/SVP/src/test/resources/datadriven/autenticacion/autenticacion.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>Orientacion</t>
   </si>
@@ -86,6 +86,24 @@
   </si>
   <si>
     <t>SVPPRU08</t>
+  </si>
+  <si>
+    <t>20513841</t>
+  </si>
+  <si>
+    <t>1989636238</t>
+  </si>
+  <si>
+    <t>USUARIOS41</t>
+  </si>
+  <si>
+    <t>MORAM12</t>
+  </si>
+  <si>
+    <t>Usuario o clave inválida. Inténtalo nuevamente</t>
+  </si>
+  <si>
+    <t>La clave que usas en el cajero está bloqueada. Debes activarla en la Sucursal Física. Para mayor información comunícate con la Sucursal Telefónica.</t>
   </si>
 </sst>
 </file>
@@ -153,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -166,6 +184,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,7 +497,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -482,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -492,7 +517,7 @@
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="139.28515625" customWidth="1"/>
     <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.7109375" customWidth="1"/>
@@ -588,15 +613,23 @@
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="1"/>
+      <c r="E5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1234</v>
+      </c>
       <c r="I5" s="1"/>
       <c r="J5" s="4"/>
     </row>
@@ -609,10 +642,16 @@
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="1"/>
+      <c r="G6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="1">
+        <v>4567</v>
+      </c>
       <c r="I6" s="1"/>
       <c r="J6" s="4"/>
     </row>
@@ -620,15 +659,21 @@
       <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="5"/>
+      <c r="E7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="G7" s="5"/>
-      <c r="H7" s="1"/>
+      <c r="H7" s="1">
+        <v>1234</v>
+      </c>
       <c r="I7" s="1"/>
       <c r="J7" s="4"/>
     </row>
@@ -641,10 +686,16 @@
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="1"/>
+      <c r="G8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1234</v>
+      </c>
       <c r="I8" s="1"/>
       <c r="J8" s="4"/>
     </row>

</xml_diff>

<commit_message>
se implementa flujos alterno del módulo de autenticación quedando pendiente la validación de los mensajes.
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/autenticacion/autenticacion.xlsx
+++ b/SVP/src/test/resources/datadriven/autenticacion/autenticacion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="13080"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
   <si>
     <t>Orientacion</t>
   </si>
@@ -85,9 +85,6 @@
     <t>7</t>
   </si>
   <si>
-    <t>SVPPRU08</t>
-  </si>
-  <si>
     <t>20513841</t>
   </si>
   <si>
@@ -97,13 +94,22 @@
     <t>USUARIOS41</t>
   </si>
   <si>
-    <t>MORAM12</t>
-  </si>
-  <si>
-    <t>Usuario o clave inválida. Inténtalo nuevamente</t>
-  </si>
-  <si>
     <t>La clave que usas en el cajero está bloqueada. Debes activarla en la Sucursal Física. Para mayor información comunícate con la Sucursal Telefónica.</t>
+  </si>
+  <si>
+    <t>OSVPPRU10</t>
+  </si>
+  <si>
+    <t>OSVPPRU04</t>
+  </si>
+  <si>
+    <t>854124014</t>
+  </si>
+  <si>
+    <t>Usuario o clave inválida. Inténtalo nuevamente.</t>
+  </si>
+  <si>
+    <t>¡Hola!</t>
   </si>
 </sst>
 </file>
@@ -497,7 +503,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -507,8 +513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -566,10 +572,12 @@
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="H2" s="1">
         <v>1234</v>
@@ -586,10 +594,16 @@
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="1"/>
+      <c r="G3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1234</v>
+      </c>
       <c r="I3" s="1"/>
       <c r="J3" s="4"/>
     </row>
@@ -619,13 +633,13 @@
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H5" s="1">
         <v>1234</v>
@@ -643,11 +657,11 @@
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H6" s="1">
         <v>4567</v>
@@ -665,10 +679,10 @@
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="1">
@@ -687,12 +701,12 @@
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5" t="s">
-        <v>24</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="5"/>
       <c r="H8" s="1">
         <v>1234</v>
       </c>

</xml_diff>

<commit_message>
se ajustan mensajes en mo´dulo de autenticación
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/autenticacion/autenticacion.xlsx
+++ b/SVP/src/test/resources/datadriven/autenticacion/autenticacion.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t>Orientacion</t>
   </si>
@@ -97,19 +97,16 @@
     <t>La clave que usas en el cajero está bloqueada. Debes activarla en la Sucursal Física. Para mayor información comunícate con la Sucursal Telefónica.</t>
   </si>
   <si>
-    <t>OSVPPRU10</t>
-  </si>
-  <si>
     <t>OSVPPRU04</t>
   </si>
   <si>
     <t>854124014</t>
   </si>
   <si>
-    <t>Usuario o clave inválida. Inténtalo nuevamente.</t>
-  </si>
-  <si>
     <t>¡Hola!</t>
+  </si>
+  <si>
+    <t>Usuario o clave inválida. Inténtalo nuevamente</t>
   </si>
 </sst>
 </file>
@@ -503,7 +500,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -513,8 +510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -573,7 +570,7 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5" t="s">
@@ -595,7 +592,7 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5" t="s">
@@ -661,7 +658,7 @@
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H6" s="1">
         <v>4567</v>
@@ -704,7 +701,7 @@
         <v>27</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="1">

</xml_diff>

<commit_message>
se trabaja sobre scritp sprint 7-8
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/autenticacion/autenticacion.xlsx
+++ b/SVP/src/test/resources/datadriven/autenticacion/autenticacion.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t>Orientacion</t>
   </si>
@@ -85,21 +85,12 @@
     <t>7</t>
   </si>
   <si>
-    <t>20513841</t>
-  </si>
-  <si>
     <t>1989636238</t>
   </si>
   <si>
-    <t>USUARIOS41</t>
-  </si>
-  <si>
     <t>La clave que usas en el cajero está bloqueada. Debes activarla en la Sucursal Física. Para mayor información comunícate con la Sucursal Telefónica.</t>
   </si>
   <si>
-    <t>OSVPPRU04</t>
-  </si>
-  <si>
     <t>854124014</t>
   </si>
   <si>
@@ -107,6 +98,21 @@
   </si>
   <si>
     <t>Usuario o clave inválida. Inténtalo nuevamente</t>
+  </si>
+  <si>
+    <t>OSVPPRU10</t>
+  </si>
+  <si>
+    <t>52269682</t>
+  </si>
+  <si>
+    <t>OSVPPRU11</t>
+  </si>
+  <si>
+    <t>OSVPPRU12</t>
+  </si>
+  <si>
+    <t>OSVPPRU01</t>
   </si>
 </sst>
 </file>
@@ -500,7 +506,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -510,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -570,11 +576,11 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H2" s="1">
         <v>1234</v>
@@ -592,11 +598,11 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="H3" s="1">
         <v>1234</v>
@@ -630,13 +636,13 @@
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H5" s="1">
         <v>1234</v>
@@ -654,11 +660,11 @@
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="H6" s="1">
         <v>4567</v>
@@ -676,10 +682,10 @@
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="1">
@@ -698,10 +704,10 @@
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="1">

</xml_diff>

<commit_message>
implementación flujo de autenticación
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/autenticacion/autenticacion.xlsx
+++ b/SVP/src/test/resources/datadriven/autenticacion/autenticacion.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>Orientacion</t>
   </si>
@@ -70,9 +70,6 @@
     <t>Alterno</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>4</t>
   </si>
   <si>
@@ -112,7 +109,7 @@
     <t>OSVPPRU12</t>
   </si>
   <si>
-    <t>OSVPPRU01</t>
+    <t>chipote87</t>
   </si>
 </sst>
 </file>
@@ -514,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -576,11 +573,11 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H2" s="1">
         <v>1234</v>
@@ -598,11 +595,11 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H3" s="1">
         <v>1234</v>
@@ -614,15 +611,23 @@
       <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="1"/>
+      <c r="E4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1234</v>
+      </c>
       <c r="I4" s="1"/>
       <c r="J4" s="4"/>
     </row>
@@ -630,22 +635,20 @@
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>1</v>
+      <c r="B5" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="H5" s="1">
-        <v>1234</v>
+        <v>4567</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="4"/>
@@ -654,20 +657,20 @@
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5" t="s">
-        <v>29</v>
-      </c>
+      <c r="E6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="5"/>
       <c r="H6" s="1">
-        <v>4567</v>
+        <v>1234</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="4"/>
@@ -676,16 +679,16 @@
       <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="1">
@@ -693,28 +696,6 @@
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="4"/>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="1">
-        <v>1234</v>
-      </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -726,7 +707,7 @@
           <x14:formula1>
             <xm:f>Listas!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B8</xm:sqref>
+          <xm:sqref>B2:B7</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
se ajusta scripts de autenticación para que valide frase, imagen y login exitoso
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/autenticacion/autenticacion.xlsx
+++ b/SVP/src/test/resources/datadriven/autenticacion/autenticacion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="44">
   <si>
     <t>Acierto</t>
   </si>
@@ -103,9 +103,6 @@
     <t>OSVPPRU11</t>
   </si>
   <si>
-    <t>OSVPPRU12</t>
-  </si>
-  <si>
     <t>OSVPPRU06</t>
   </si>
   <si>
@@ -152,6 +149,12 @@
   </si>
   <si>
     <t>OSVPPRU24</t>
+  </si>
+  <si>
+    <t>chipote25</t>
+  </si>
+  <si>
+    <t>Hola</t>
   </si>
 </sst>
 </file>
@@ -555,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:J8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -615,7 +618,7 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5" t="s">
@@ -637,11 +640,11 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="H3" s="1">
         <v>1234</v>
@@ -651,7 +654,7 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>0</v>
@@ -687,7 +690,7 @@
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H5" s="1">
         <v>4567</v>
@@ -731,7 +734,7 @@
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H7" s="1">
         <v>1234</v>
@@ -783,7 +786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -837,7 +840,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -851,7 +854,7 @@
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -859,7 +862,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -868,14 +871,14 @@
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H3" s="1">
         <v>1234</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -883,7 +886,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -897,7 +900,7 @@
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -914,14 +917,14 @@
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H5" s="1">
         <v>1234</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="41.25" customHeight="1">
@@ -938,14 +941,14 @@
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H6" s="1">
         <v>1234</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -965,7 +968,7 @@
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -987,7 +990,7 @@
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1009,7 +1012,7 @@
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1031,7 +1034,7 @@
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>